<commit_message>
adding precision statement for nutrients
</commit_message>
<xml_diff>
--- a/Data/Biogeochem/RawNutrientData/TidePoolNutrientsQAQC.xlsx
+++ b/Data/Biogeochem/RawNutrientData/TidePoolNutrientsQAQC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferfields/Desktop/OregonSummer2019/IntertidalFoundationSpeciesEcoFun/Data/Biogeochemistry/RawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferfields/Desktop/OregonSummer2019/EcoFunORTidepools/Data/Biogeochem/RawNutrientData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAB785C-7F2F-A244-B9FE-2B76B72AE980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62062657-BF59-3349-89A6-8D1167D50BE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="25060" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4041" uniqueCount="741">
   <si>
     <t>Id_code</t>
   </si>
@@ -2258,6 +2258,177 @@
   </si>
   <si>
     <t>N_16_5_AI</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">± </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.21% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, ± </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">0.26% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">− </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+ NO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>−</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, ± 3.57% PO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> − </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>instrument precision</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2267,7 +2438,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2330,6 +2501,41 @@
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2563,7 +2769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2836,6 +3042,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31319,8 +31526,8 @@
   </sheetPr>
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -31927,7 +32134,9 @@
         <v>27</v>
       </c>
       <c r="G24" s="55"/>
-      <c r="H24" s="7"/>
+      <c r="H24" s="128" t="s">
+        <v>740</v>
+      </c>
       <c r="I24" s="7"/>
       <c r="J24" s="56"/>
       <c r="K24" s="56"/>
@@ -31938,7 +32147,7 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" ht="16">
       <c r="A25" s="57" t="s">
         <v>51</v>
       </c>

</xml_diff>